<commit_message>
Anpassungen nach Sitzung 19.12
</commit_message>
<xml_diff>
--- a/Tabellen/BIvariate.xlsx
+++ b/Tabellen/BIvariate.xlsx
@@ -589,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>34.37</v>
+        <v>34.38</v>
       </c>
       <c r="D6" t="n">
         <v>19.7</v>
@@ -601,7 +601,7 @@
         <v>33.65</v>
       </c>
       <c r="G6" t="n">
-        <v>39.25</v>
+        <v>39.27</v>
       </c>
       <c r="H6" t="n">
         <v>55.1</v>
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>35.07</v>
+        <v>35.09</v>
       </c>
       <c r="D7" t="n">
         <v>21.3</v>
@@ -630,16 +630,16 @@
         <v>30.6</v>
       </c>
       <c r="F7" t="n">
-        <v>34.8</v>
+        <v>34.7</v>
       </c>
       <c r="G7" t="n">
-        <v>40.2</v>
+        <v>40.1</v>
       </c>
       <c r="H7" t="n">
         <v>49.7</v>
       </c>
       <c r="I7" t="n">
-        <v>5.92</v>
+        <v>5.94</v>
       </c>
       <c r="J7" t="n">
         <v>61</v>

</xml_diff>